<commit_message>
addition of builds and plugins
</commit_message>
<xml_diff>
--- a/testData/AsiData_615.xlsx
+++ b/testData/AsiData_615.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\webca\eclipse-workspace\Framework2\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE48E20-C3DC-4185-9265-2FD8E564CCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C5E1D8-A88C-4D68-B0EE-76CBA35B1806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D49CA3B2-E4C4-4306-82E9-CD7D81BF161A}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>OpenWidth</t>
   </si>
   <si>
-    <t xml:space="preserve">Price </t>
-  </si>
-  <si>
     <t>Brand</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>FABRICDOOR</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -507,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F8A7DF-1A91-4F51-ABFB-5F2AFDA32997}">
-  <dimension ref="A1:E241"/>
+  <dimension ref="A1:H241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="I135" sqref="I135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,10 +522,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>0</v>
@@ -533,13 +533,11 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="9">
         <v>615</v>
@@ -556,7 +554,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="9">
         <v>615</v>
@@ -573,7 +571,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="9">
         <v>615</v>
@@ -590,7 +588,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="9">
         <v>615</v>
@@ -607,7 +605,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="9">
         <v>615</v>
@@ -624,7 +622,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="9">
         <v>615</v>
@@ -641,7 +639,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="9">
         <v>615</v>
@@ -658,7 +656,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="9">
         <v>615</v>
@@ -675,7 +673,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="9">
         <v>615</v>
@@ -692,7 +690,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="9">
         <v>615</v>
@@ -709,7 +707,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="9">
         <v>615</v>
@@ -726,7 +724,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="9">
         <v>615</v>
@@ -743,7 +741,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="9">
         <v>615</v>
@@ -760,7 +758,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="9">
         <v>615</v>
@@ -777,7 +775,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="9">
         <v>615</v>
@@ -794,7 +792,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="9">
         <v>615</v>
@@ -811,7 +809,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="9">
         <v>615</v>
@@ -828,7 +826,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="9">
         <v>615</v>
@@ -845,7 +843,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="9">
         <v>615</v>
@@ -862,7 +860,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="9">
         <v>615</v>
@@ -879,7 +877,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="9">
         <v>615</v>
@@ -896,7 +894,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="9">
         <v>615</v>
@@ -913,7 +911,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="9">
         <v>615</v>
@@ -930,7 +928,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="9">
         <v>615</v>
@@ -947,7 +945,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" s="9">
         <v>615</v>
@@ -964,7 +962,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27" s="9">
         <v>615</v>
@@ -981,7 +979,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" s="9">
         <v>615</v>
@@ -998,7 +996,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B29" s="9">
         <v>615</v>
@@ -1015,7 +1013,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B30" s="9">
         <v>615</v>
@@ -1032,7 +1030,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31" s="9">
         <v>615</v>
@@ -1049,7 +1047,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B32" s="9">
         <v>615</v>
@@ -1061,12 +1059,12 @@
         <v>5</v>
       </c>
       <c r="E32" s="1">
-        <v>10839.999999999998</v>
+        <v>10690.333333333332</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B33" s="9">
         <v>615</v>
@@ -1078,12 +1076,12 @@
         <v>5</v>
       </c>
       <c r="E33" s="1">
-        <v>11084.62857142857</v>
+        <v>10928.704761904761</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B34" s="9">
         <v>615</v>
@@ -1095,12 +1093,12 @@
         <v>5</v>
       </c>
       <c r="E34" s="1">
-        <v>11329.257142857141</v>
+        <v>11167.076190476189</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B35" s="9">
         <v>615</v>
@@ -1112,12 +1110,12 @@
         <v>5</v>
       </c>
       <c r="E35" s="2">
-        <v>11573.885714285712</v>
+        <v>11405.447619047618</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36" s="9">
         <v>615</v>
@@ -1129,12 +1127,12 @@
         <v>5</v>
       </c>
       <c r="E36" s="2">
-        <v>11818.514285714284</v>
+        <v>11643.819047619047</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B37" s="9">
         <v>615</v>
@@ -1146,12 +1144,12 @@
         <v>5</v>
       </c>
       <c r="E37" s="2">
-        <v>12063.142857142855</v>
+        <v>11882.190476190475</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B38" s="9">
         <v>615</v>
@@ -1163,12 +1161,12 @@
         <v>5</v>
       </c>
       <c r="E38" s="2">
-        <v>12307.771428571426</v>
+        <v>12120.561904761904</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B39" s="9">
         <v>615</v>
@@ -1180,12 +1178,12 @@
         <v>5</v>
       </c>
       <c r="E39" s="2">
-        <v>12552.399999999998</v>
+        <v>12358.933333333332</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B40" s="9">
         <v>615</v>
@@ -1197,12 +1195,12 @@
         <v>5</v>
       </c>
       <c r="E40" s="2">
-        <v>12797.028571428569</v>
+        <v>12597.304761904761</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B41" s="9">
         <v>615</v>
@@ -1214,12 +1212,12 @@
         <v>5</v>
       </c>
       <c r="E41" s="2">
-        <v>13041.657142857141</v>
+        <v>12835.67619047619</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B42" s="9">
         <v>615</v>
@@ -1231,12 +1229,12 @@
         <v>5</v>
       </c>
       <c r="E42" s="2">
-        <v>13286.285714285712</v>
+        <v>13074.047619047618</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B43" s="9">
         <v>615</v>
@@ -1248,12 +1246,12 @@
         <v>5</v>
       </c>
       <c r="E43" s="2">
-        <v>13530.914285714283</v>
+        <v>13312.419047619047</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B44" s="9">
         <v>615</v>
@@ -1265,12 +1263,12 @@
         <v>5</v>
       </c>
       <c r="E44" s="2">
-        <v>13775.542857142855</v>
+        <v>13550.790476190476</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B45" s="9">
         <v>615</v>
@@ -1282,12 +1280,12 @@
         <v>5</v>
       </c>
       <c r="E45" s="2">
-        <v>14020.171428571426</v>
+        <v>13789.161904761904</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B46" s="9">
         <v>615</v>
@@ -1299,12 +1297,12 @@
         <v>5</v>
       </c>
       <c r="E46" s="2">
-        <v>14264.8</v>
+        <v>14027.533333333333</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B47" s="9">
         <v>615</v>
@@ -1321,7 +1319,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B48" s="9">
         <v>615</v>
@@ -1338,7 +1336,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B49" s="9">
         <v>615</v>
@@ -1355,7 +1353,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B50" s="9">
         <v>615</v>
@@ -1372,7 +1370,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B51" s="9">
         <v>615</v>
@@ -1389,7 +1387,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B52" s="9">
         <v>615</v>
@@ -1406,7 +1404,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B53" s="9">
         <v>615</v>
@@ -1423,7 +1421,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B54" s="9">
         <v>615</v>
@@ -1440,7 +1438,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B55" s="9">
         <v>615</v>
@@ -1457,7 +1455,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B56" s="9">
         <v>615</v>
@@ -1474,7 +1472,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B57" s="9">
         <v>615</v>
@@ -1491,7 +1489,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B58" s="9">
         <v>615</v>
@@ -1503,12 +1501,12 @@
         <v>6</v>
       </c>
       <c r="E58" s="2">
-        <v>13530.9142857143</v>
+        <v>13530.914285714283</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B59" s="9">
         <v>615</v>
@@ -1525,7 +1523,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B60" s="9">
         <v>615</v>
@@ -1542,7 +1540,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B61" s="9">
         <v>615</v>
@@ -1559,7 +1557,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B62" s="9">
         <v>615</v>
@@ -1576,7 +1574,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B63" s="9">
         <v>615</v>
@@ -1593,7 +1591,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B64" s="9">
         <v>615</v>
@@ -1610,7 +1608,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B65" s="9">
         <v>615</v>
@@ -1627,7 +1625,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B66" s="9">
         <v>615</v>
@@ -1644,7 +1642,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B67" s="9">
         <v>615</v>
@@ -1661,7 +1659,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B68" s="9">
         <v>615</v>
@@ -1678,7 +1676,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B69" s="9">
         <v>615</v>
@@ -1695,7 +1693,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B70" s="9">
         <v>615</v>
@@ -1712,7 +1710,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B71" s="9">
         <v>615</v>
@@ -1729,7 +1727,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B72" s="9">
         <v>615</v>
@@ -1746,7 +1744,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B73" s="9">
         <v>615</v>
@@ -1763,7 +1761,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B74" s="9">
         <v>615</v>
@@ -1780,7 +1778,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B75" s="9">
         <v>615</v>
@@ -1797,7 +1795,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B76" s="9">
         <v>615</v>
@@ -1814,7 +1812,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B77" s="9">
         <v>615</v>
@@ -1831,7 +1829,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B78" s="9">
         <v>615</v>
@@ -1848,7 +1846,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B79" s="9">
         <v>615</v>
@@ -1865,7 +1863,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B80" s="9">
         <v>615</v>
@@ -1882,7 +1880,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B81" s="9">
         <v>615</v>
@@ -1899,7 +1897,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B82" s="9">
         <v>615</v>
@@ -1916,7 +1914,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B83" s="9">
         <v>615</v>
@@ -1933,7 +1931,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B84" s="9">
         <v>615</v>
@@ -1950,7 +1948,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B85" s="9">
         <v>615</v>
@@ -1967,7 +1965,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B86" s="9">
         <v>615</v>
@@ -1984,7 +1982,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B87" s="9">
         <v>615</v>
@@ -2001,7 +1999,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B88" s="9">
         <v>615</v>
@@ -2018,7 +2016,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B89" s="9">
         <v>615</v>
@@ -2035,7 +2033,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B90" s="9">
         <v>615</v>
@@ -2052,7 +2050,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B91" s="9">
         <v>615</v>
@@ -2069,7 +2067,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B92" s="9">
         <v>615</v>
@@ -2086,7 +2084,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B93" s="9">
         <v>615</v>
@@ -2103,7 +2101,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B94" s="9">
         <v>615</v>
@@ -2120,7 +2118,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B95" s="9">
         <v>615</v>
@@ -2137,7 +2135,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B96" s="9">
         <v>615</v>
@@ -2154,7 +2152,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B97" s="9">
         <v>615</v>
@@ -2171,7 +2169,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B98" s="9">
         <v>615</v>
@@ -2188,7 +2186,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B99" s="9">
         <v>615</v>
@@ -2205,7 +2203,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B100" s="9">
         <v>615</v>
@@ -2222,7 +2220,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B101" s="9">
         <v>615</v>
@@ -2239,7 +2237,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B102" s="9">
         <v>615</v>
@@ -2256,7 +2254,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B103" s="9">
         <v>615</v>
@@ -2273,7 +2271,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B104" s="9">
         <v>615</v>
@@ -2290,7 +2288,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B105" s="9">
         <v>615</v>
@@ -2307,7 +2305,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B106" s="9">
         <v>615</v>
@@ -2324,7 +2322,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B107" s="9">
         <v>615</v>
@@ -2341,7 +2339,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B108" s="9">
         <v>615</v>
@@ -2358,7 +2356,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B109" s="9">
         <v>615</v>
@@ -2375,7 +2373,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B110" s="9">
         <v>615</v>
@@ -2392,7 +2390,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B111" s="9">
         <v>615</v>
@@ -2409,7 +2407,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B112" s="9">
         <v>615</v>
@@ -2426,7 +2424,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B113" s="9">
         <v>615</v>
@@ -2443,7 +2441,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B114" s="9">
         <v>615</v>
@@ -2460,7 +2458,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B115" s="9">
         <v>615</v>
@@ -2477,7 +2475,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B116" s="9">
         <v>615</v>
@@ -2494,7 +2492,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B117" s="9">
         <v>615</v>
@@ -2511,7 +2509,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B118" s="9">
         <v>615</v>
@@ -2528,7 +2526,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B119" s="9">
         <v>615</v>
@@ -2545,7 +2543,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B120" s="9">
         <v>615</v>
@@ -2562,7 +2560,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B121" s="9">
         <v>615</v>
@@ -2579,7 +2577,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B122" s="9">
         <v>615</v>
@@ -2590,13 +2588,13 @@
       <c r="D122" s="6">
         <v>11</v>
       </c>
-      <c r="E122" s="10">
-        <v>11737.999999999995</v>
+      <c r="E122" s="1">
+        <v>11588.333333333328</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B123" s="9">
         <v>615</v>
@@ -2607,13 +2605,13 @@
       <c r="D123" s="6">
         <v>11</v>
       </c>
-      <c r="E123" s="10">
-        <v>12020.171428571422</v>
+      <c r="E123" s="1">
+        <v>11864.247619047614</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B124" s="9">
         <v>615</v>
@@ -2624,13 +2622,13 @@
       <c r="D124" s="6">
         <v>11</v>
       </c>
-      <c r="E124" s="10">
-        <v>12302.342857142852</v>
+      <c r="E124" s="1">
+        <v>12140.161904761899</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B125" s="9">
         <v>615</v>
@@ -2642,12 +2640,12 @@
         <v>11</v>
       </c>
       <c r="E125" s="2">
-        <v>12584.514285714282</v>
+        <v>12416.076190476184</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B126" s="9">
         <v>615</v>
@@ -2659,12 +2657,12 @@
         <v>11</v>
       </c>
       <c r="E126" s="2">
-        <v>12866.685714285712</v>
+        <v>12691.990476190469</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B127" s="9">
         <v>615</v>
@@ -2676,12 +2674,12 @@
         <v>11</v>
       </c>
       <c r="E127" s="2">
-        <v>13148.857142857141</v>
+        <v>12967.904761904754</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B128" s="9">
         <v>615</v>
@@ -2693,12 +2691,12 @@
         <v>11</v>
       </c>
       <c r="E128" s="2">
-        <v>13431.028571428571</v>
+        <v>13243.819047619039</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B129" s="9">
         <v>615</v>
@@ -2710,12 +2708,12 @@
         <v>11</v>
       </c>
       <c r="E129" s="2">
-        <v>13713.2</v>
+        <v>13519.733333333324</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B130" s="9">
         <v>615</v>
@@ -2727,12 +2725,12 @@
         <v>11</v>
       </c>
       <c r="E130" s="2">
-        <v>13995.37142857143</v>
+        <v>13795.64761904761</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B131" s="9">
         <v>615</v>
@@ -2744,12 +2742,12 @@
         <v>11</v>
       </c>
       <c r="E131" s="2">
-        <v>14277.54285714286</v>
+        <v>14071.561904761895</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B132" s="9">
         <v>615</v>
@@ -2761,12 +2759,12 @@
         <v>11</v>
       </c>
       <c r="E132" s="2">
-        <v>14559.71428571429</v>
+        <v>14347.47619047618</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B133" s="9">
         <v>615</v>
@@ -2778,12 +2776,12 @@
         <v>11</v>
       </c>
       <c r="E133" s="2">
-        <v>14841.88571428572</v>
+        <v>14623.390476190465</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B134" s="9">
         <v>615</v>
@@ -2795,12 +2793,12 @@
         <v>11</v>
       </c>
       <c r="E134" s="2">
-        <v>15124.057142857149</v>
+        <v>14899.30476190475</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B135" s="9">
         <v>615</v>
@@ -2812,12 +2810,12 @@
         <v>11</v>
       </c>
       <c r="E135" s="2">
-        <v>15406.228571428579</v>
+        <v>15175.219047619035</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B136" s="9">
         <v>615</v>
@@ -2829,12 +2827,12 @@
         <v>11</v>
       </c>
       <c r="E136" s="2">
-        <v>15688.399999999998</v>
+        <v>15451.133333333331</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B137" s="9">
         <v>615</v>
@@ -2851,7 +2849,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B138" s="9">
         <v>615</v>
@@ -2868,7 +2866,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B139" s="9">
         <v>615</v>
@@ -2885,7 +2883,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B140" s="9">
         <v>615</v>
@@ -2902,7 +2900,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B141" s="9">
         <v>615</v>
@@ -2919,7 +2917,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B142" s="9">
         <v>615</v>
@@ -2936,7 +2934,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B143" s="9">
         <v>615</v>
@@ -2953,7 +2951,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B144" s="9">
         <v>615</v>
@@ -2970,7 +2968,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B145" s="9">
         <v>615</v>
@@ -2987,7 +2985,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B146" s="9">
         <v>615</v>
@@ -3004,7 +3002,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B147" s="9">
         <v>615</v>
@@ -3021,7 +3019,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B148" s="9">
         <v>615</v>
@@ -3038,7 +3036,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B149" s="9">
         <v>615</v>
@@ -3055,7 +3053,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B150" s="9">
         <v>615</v>
@@ -3072,7 +3070,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B151" s="9">
         <v>615</v>
@@ -3089,7 +3087,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B152" s="9">
         <v>615</v>
@@ -3106,7 +3104,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B153" s="9">
         <v>615</v>
@@ -3123,7 +3121,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B154" s="9">
         <v>615</v>
@@ -3140,7 +3138,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B155" s="9">
         <v>615</v>
@@ -3157,7 +3155,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B156" s="9">
         <v>615</v>
@@ -3174,7 +3172,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B157" s="9">
         <v>615</v>
@@ -3191,7 +3189,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B158" s="9">
         <v>615</v>
@@ -3208,7 +3206,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B159" s="9">
         <v>615</v>
@@ -3225,7 +3223,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B160" s="9">
         <v>615</v>
@@ -3242,7 +3240,7 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B161" s="9">
         <v>615</v>
@@ -3259,7 +3257,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B162" s="9">
         <v>615</v>
@@ -3276,7 +3274,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B163" s="9">
         <v>615</v>
@@ -3293,7 +3291,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B164" s="9">
         <v>615</v>
@@ -3310,7 +3308,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B165" s="9">
         <v>615</v>
@@ -3327,7 +3325,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B166" s="9">
         <v>615</v>
@@ -3344,7 +3342,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B167" s="9">
         <v>615</v>
@@ -3361,7 +3359,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B168" s="9">
         <v>615</v>
@@ -3378,7 +3376,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B169" s="9">
         <v>615</v>
@@ -3395,7 +3393,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B170" s="9">
         <v>615</v>
@@ -3412,7 +3410,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B171" s="9">
         <v>615</v>
@@ -3429,7 +3427,7 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B172" s="9">
         <v>615</v>
@@ -3446,7 +3444,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B173" s="9">
         <v>615</v>
@@ -3463,7 +3461,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B174" s="9">
         <v>615</v>
@@ -3480,7 +3478,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B175" s="9">
         <v>615</v>
@@ -3497,7 +3495,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B176" s="9">
         <v>615</v>
@@ -3514,7 +3512,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B177" s="9">
         <v>615</v>
@@ -3531,7 +3529,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B178" s="9">
         <v>615</v>
@@ -3548,7 +3546,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B179" s="9">
         <v>615</v>
@@ -3565,7 +3563,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B180" s="9">
         <v>615</v>
@@ -3582,7 +3580,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B181" s="9">
         <v>615</v>
@@ -3599,7 +3597,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B182" s="9">
         <v>615</v>
@@ -3611,12 +3609,12 @@
         <v>15</v>
       </c>
       <c r="E182" s="1">
-        <v>12336.666666666659</v>
+        <v>12186.999999999993</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B183" s="9">
         <v>615</v>
@@ -3628,12 +3626,12 @@
         <v>15</v>
       </c>
       <c r="E183" s="1">
-        <v>12643.86666666666</v>
+        <v>12487.942857142851</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B184" s="9">
         <v>615</v>
@@ -3645,12 +3643,12 @@
         <v>15</v>
       </c>
       <c r="E184" s="1">
-        <v>12951.06666666666</v>
+        <v>12788.885714285709</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B185" s="9">
         <v>615</v>
@@ -3662,12 +3660,12 @@
         <v>15</v>
       </c>
       <c r="E185" s="2">
-        <v>13258.266666666661</v>
+        <v>13089.828571428567</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B186" s="9">
         <v>615</v>
@@ -3679,12 +3677,12 @@
         <v>15</v>
       </c>
       <c r="E186" s="2">
-        <v>13565.466666666662</v>
+        <v>13390.771428571425</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B187" s="9">
         <v>615</v>
@@ -3696,12 +3694,12 @@
         <v>15</v>
       </c>
       <c r="E187" s="2">
-        <v>13872.666666666662</v>
+        <v>13691.714285714283</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B188" s="9">
         <v>615</v>
@@ -3713,12 +3711,12 @@
         <v>15</v>
       </c>
       <c r="E188" s="2">
-        <v>14179.866666666663</v>
+        <v>13992.657142857141</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B189" s="9">
         <v>615</v>
@@ -3730,12 +3728,12 @@
         <v>15</v>
       </c>
       <c r="E189" s="2">
-        <v>14487.066666666664</v>
+        <v>14293.599999999999</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B190" s="9">
         <v>615</v>
@@ -3747,12 +3745,12 @@
         <v>15</v>
       </c>
       <c r="E190" s="2">
-        <v>14794.266666666665</v>
+        <v>14594.542857142857</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B191" s="9">
         <v>615</v>
@@ -3764,12 +3762,12 @@
         <v>15</v>
       </c>
       <c r="E191" s="2">
-        <v>15101.466666666665</v>
+        <v>14895.485714285714</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B192" s="9">
         <v>615</v>
@@ -3781,12 +3779,12 @@
         <v>15</v>
       </c>
       <c r="E192" s="2">
-        <v>15408.666666666666</v>
+        <v>15196.428571428572</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B193" s="9">
         <v>615</v>
@@ -3798,12 +3796,12 @@
         <v>15</v>
       </c>
       <c r="E193" s="2">
-        <v>15715.866666666667</v>
+        <v>15497.37142857143</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B194" s="9">
         <v>615</v>
@@ -3815,12 +3813,12 @@
         <v>15</v>
       </c>
       <c r="E194" s="2">
-        <v>16023.066666666668</v>
+        <v>15798.314285714288</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B195" s="9">
         <v>615</v>
@@ -3832,12 +3830,12 @@
         <v>15</v>
       </c>
       <c r="E195" s="2">
-        <v>16330.266666666668</v>
+        <v>16099.257142857146</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B196" s="9">
         <v>615</v>
@@ -3849,12 +3847,12 @@
         <v>15</v>
       </c>
       <c r="E196" s="2">
-        <v>16637.466666666664</v>
+        <v>16400.199999999997</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B197" s="9">
         <v>615</v>
@@ -3871,7 +3869,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B198" s="9">
         <v>615</v>
@@ -3888,7 +3886,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B199" s="9">
         <v>615</v>
@@ -3905,7 +3903,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B200" s="9">
         <v>615</v>
@@ -3922,7 +3920,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B201" s="9">
         <v>615</v>
@@ -3939,7 +3937,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B202" s="9">
         <v>615</v>
@@ -3956,7 +3954,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B203" s="9">
         <v>615</v>
@@ -3973,7 +3971,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B204" s="9">
         <v>615</v>
@@ -3990,7 +3988,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B205" s="9">
         <v>615</v>
@@ -4007,7 +4005,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B206" s="9">
         <v>615</v>
@@ -4024,7 +4022,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B207" s="9">
         <v>615</v>
@@ -4041,7 +4039,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B208" s="9">
         <v>615</v>
@@ -4056,9 +4054,9 @@
         <v>15715.866666666667</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B209" s="9">
         <v>615</v>
@@ -4073,9 +4071,9 @@
         <v>16023.066666666668</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B210" s="9">
         <v>615</v>
@@ -4090,9 +4088,9 @@
         <v>16330.266666666668</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B211" s="9">
         <v>615</v>
@@ -4107,9 +4105,9 @@
         <v>16637.466666666664</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B212" s="9">
         <v>615</v>
@@ -4121,12 +4119,12 @@
         <v>17</v>
       </c>
       <c r="E212" s="1">
-        <v>12636</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+        <v>12486.333333333325</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B213" s="9">
         <v>615</v>
@@ -4138,12 +4136,12 @@
         <v>17</v>
       </c>
       <c r="E213" s="1">
-        <v>12955.714285714286</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+        <v>12799.790476190468</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B214" s="9">
         <v>615</v>
@@ -4155,12 +4153,15 @@
         <v>17</v>
       </c>
       <c r="E214" s="1">
-        <v>13275.428571428572</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13113.247619047612</v>
+      </c>
+      <c r="H214" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B215" s="9">
         <v>615</v>
@@ -4172,12 +4173,12 @@
         <v>17</v>
       </c>
       <c r="E215" s="2">
-        <v>13595.142857142859</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13426.704761904755</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B216" s="9">
         <v>615</v>
@@ -4189,12 +4190,12 @@
         <v>17</v>
       </c>
       <c r="E216" s="2">
-        <v>13914.857142857145</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13740.161904761899</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B217" s="9">
         <v>615</v>
@@ -4206,12 +4207,12 @@
         <v>17</v>
       </c>
       <c r="E217" s="2">
-        <v>14234.571428571431</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14053.619047619042</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B218" s="9">
         <v>615</v>
@@ -4223,12 +4224,12 @@
         <v>17</v>
       </c>
       <c r="E218" s="2">
-        <v>14554.285714285717</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14367.076190476186</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B219" s="9">
         <v>615</v>
@@ -4240,12 +4241,12 @@
         <v>17</v>
       </c>
       <c r="E219" s="2">
-        <v>14874.000000000004</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14680.533333333329</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B220" s="9">
         <v>615</v>
@@ -4257,12 +4258,12 @@
         <v>17</v>
       </c>
       <c r="E220" s="2">
-        <v>15193.71428571429</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14993.990476190473</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B221" s="9">
         <v>615</v>
@@ -4274,12 +4275,12 @@
         <v>17</v>
       </c>
       <c r="E221" s="2">
-        <v>15513.428571428576</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15307.447619047616</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B222" s="9">
         <v>615</v>
@@ -4291,12 +4292,12 @@
         <v>17</v>
       </c>
       <c r="E222" s="2">
-        <v>15833.142857142862</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15620.90476190476</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B223" s="9">
         <v>615</v>
@@ -4308,12 +4309,12 @@
         <v>17</v>
       </c>
       <c r="E223" s="2">
-        <v>16152.857142857149</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15934.361904761903</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B224" s="9">
         <v>615</v>
@@ -4325,12 +4326,12 @@
         <v>17</v>
       </c>
       <c r="E224" s="2">
-        <v>16472.571428571435</v>
+        <v>16247.819047619047</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B225" s="9">
         <v>615</v>
@@ -4342,12 +4343,12 @@
         <v>17</v>
       </c>
       <c r="E225" s="2">
-        <v>16792.285714285721</v>
+        <v>16561.27619047619</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B226" s="9">
         <v>615</v>
@@ -4359,12 +4360,12 @@
         <v>17</v>
       </c>
       <c r="E226" s="2">
-        <v>17112</v>
+        <v>16874.73333333333</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B227" s="9">
         <v>615</v>
@@ -4381,7 +4382,7 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B228" s="9">
         <v>615</v>
@@ -4398,7 +4399,7 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B229" s="9">
         <v>615</v>
@@ -4415,7 +4416,7 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B230" s="9">
         <v>615</v>
@@ -4432,7 +4433,7 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B231" s="9">
         <v>615</v>
@@ -4449,7 +4450,7 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B232" s="9">
         <v>615</v>
@@ -4466,7 +4467,7 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B233" s="9">
         <v>615</v>
@@ -4483,7 +4484,7 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B234" s="9">
         <v>615</v>
@@ -4500,7 +4501,7 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B235" s="9">
         <v>615</v>
@@ -4517,7 +4518,7 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B236" s="9">
         <v>615</v>
@@ -4534,7 +4535,7 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B237" s="9">
         <v>615</v>
@@ -4551,7 +4552,7 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B238" s="9">
         <v>615</v>
@@ -4568,7 +4569,7 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B239" s="9">
         <v>615</v>
@@ -4585,7 +4586,7 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B240" s="9">
         <v>615</v>
@@ -4602,7 +4603,7 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B241" s="9">
         <v>615</v>

</xml_diff>